<commit_message>
feat(generate_excel_from_csv): add comments to label cells with content text
Add comments to LABEL cells containing the content text from the associated file. This improves traceability by showing the full content as a comment when hovering over the label.
</commit_message>
<xml_diff>
--- a/InterviewTemplates/Interviews/InterviewTemplate.xlsx
+++ b/InterviewTemplates/Interviews/InterviewTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juangarcia/Developer/developer-roadmap/Interviews/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juangarcia/Developer/developer-roadmap/InterviewTemplates/Interviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1980A34C-39F0-6C4B-BAE8-44D3BD66A39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7381E99-2BE6-EF43-9B25-0CC994B6DDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="50880" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Score:</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>score [-100,+100]</t>
-  </si>
-  <si>
-    <t>CONTENT</t>
   </si>
 </sst>
 </file>
@@ -138,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -168,9 +165,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -524,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AB7478-9D76-6446-8BCF-DE90232840EB}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="238" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -538,10 +532,9 @@
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -559,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -581,11 +574,8 @@
       <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -606,9 +596,8 @@
         <v>1</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -818,18 +807,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,18 +841,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B308FA45-0AE6-43F7-9029-8EA8831C1DE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{263A09E4-E086-4519-B695-30CD6D1947AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B308FA45-0AE6-43F7-9029-8EA8831C1DE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>